<commit_message>
Uploading again - Jenkins results are a bit different to mine. Unsure why!
</commit_message>
<xml_diff>
--- a/Tests/Validation/System/NZRiskIndexTool/RITTemplate2025_7740Obs.xlsx
+++ b/Tests/Validation/System/NZRiskIndexTool/RITTemplate2025_7740Obs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaUnderVC\ApsimX\Tests\Validation\System\NZRiskIndexTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4232FAE7-974E-40D1-9674-D7D68658F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E6EA7C-CF12-4342-931F-770392387F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="630" windowWidth="38940" windowHeight="19095" xr2:uid="{EF6CDDDD-7646-4185-8460-A519E6392745}"/>
+    <workbookView xWindow="3900" yWindow="1785" windowWidth="38940" windowHeight="19095" xr2:uid="{EF6CDDDD-7646-4185-8460-A519E6392745}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarked2025" sheetId="1" r:id="rId1"/>
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:X217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:X217"/>
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>